<commit_message>
updated Manoj Vasala Calendar code
</commit_message>
<xml_diff>
--- a/bin/com/testdata/DataDriveTest.xlsx
+++ b/bin/com/testdata/DataDriveTest.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1D89F-7F19-491C-8F1C-AE1E9344900E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{136A70A5-BE46-4501-AC9D-856343C4A854}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId2"/>
+    <sheet name="RegTestData" r:id="rId1" sheetId="1"/>
+    <sheet name="HomePage" r:id="rId2" sheetId="2"/>
+    <sheet name="TableData" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>firstname</t>
   </si>
@@ -108,12 +109,55 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Alfreds Futterkiste</t>
+  </si>
+  <si>
+    <t>Maria Anders</t>
+  </si>
+  <si>
+    <t>Centro comercial Moctezuma</t>
+  </si>
+  <si>
+    <t>Francisco Chang</t>
+  </si>
+  <si>
+    <t>Ernst Handel</t>
+  </si>
+  <si>
+    <t>Roland Mendel</t>
+  </si>
+  <si>
+    <t>Island Trading</t>
+  </si>
+  <si>
+    <t>Helen Bennett</t>
+  </si>
+  <si>
+    <t>Laughing Bacchus Winecellars</t>
+  </si>
+  <si>
+    <t>Yoshi Tannamuri</t>
+  </si>
+  <si>
+    <t>Magazzini Alimentari Riuniti</t>
+  </si>
+  <si>
+    <t>Giovanni Rovelli</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +186,26 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
@@ -160,19 +224,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -189,10 +255,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -227,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +328,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -356,21 +422,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,7 +453,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -439,15 +505,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -455,12 +521,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.40625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.40625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.86328125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.40625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.40625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.86328125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.75">
@@ -609,19 +675,94 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.765625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.96484375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>